<commit_message>
redo norms for four TOD C scores
</commit_message>
<xml_diff>
--- a/OUTPUT-FILES/NORMS/TODC_final_gr1_12_10.28.21_fornorms/bln_sum-raw-ss-lookup-tabbed-age.xlsx
+++ b/OUTPUT-FILES/NORMS/TODC_final_gr1_12_10.28.21_fornorms/bln_sum-raw-ss-lookup-tabbed-age.xlsx
@@ -465,7 +465,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12">
@@ -473,7 +473,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13">
@@ -481,7 +481,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="14">
@@ -489,7 +489,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="15">
@@ -497,7 +497,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="16">
@@ -505,7 +505,7 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="17">
@@ -513,7 +513,7 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="18">
@@ -537,7 +537,7 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="21">
@@ -545,7 +545,7 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="22">
@@ -553,7 +553,7 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="23">
@@ -561,7 +561,7 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>122</v>
+        <v>124</v>
       </c>
     </row>
     <row r="24">
@@ -569,7 +569,7 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="25">
@@ -577,7 +577,7 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="26">
@@ -730,7 +730,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12">
@@ -738,7 +738,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="13">
@@ -746,7 +746,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="14">
@@ -754,7 +754,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="15">
@@ -762,7 +762,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="16">
@@ -770,7 +770,7 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="17">
@@ -778,7 +778,7 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="18">
@@ -786,7 +786,7 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="19">
@@ -794,7 +794,7 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="20">
@@ -802,7 +802,7 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="21">
@@ -810,7 +810,7 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="22">
@@ -818,7 +818,7 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="23">
@@ -826,7 +826,7 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="24">
@@ -834,7 +834,7 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="25">
@@ -842,7 +842,7 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="26">
@@ -850,7 +850,7 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="27">
@@ -866,7 +866,7 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="29">
@@ -995,7 +995,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12">
@@ -1003,7 +1003,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="13">
@@ -1011,7 +1011,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14">
@@ -1019,7 +1019,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="15">
@@ -1027,7 +1027,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="16">
@@ -1059,7 +1059,7 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="20">
@@ -1067,7 +1067,7 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="21">
@@ -1075,7 +1075,7 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="22">
@@ -1083,7 +1083,7 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="23">
@@ -1091,7 +1091,7 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="24">
@@ -1099,7 +1099,7 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="25">
@@ -1107,7 +1107,7 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="26">
@@ -1115,7 +1115,7 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="27">
@@ -1123,7 +1123,7 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="28">
@@ -1131,7 +1131,7 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="29">
@@ -1260,7 +1260,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12">
@@ -1268,7 +1268,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13">
@@ -1276,7 +1276,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14">
@@ -1284,7 +1284,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="15">
@@ -1292,7 +1292,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="16">
@@ -1316,7 +1316,7 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="19">
@@ -1332,7 +1332,7 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="21">
@@ -1340,7 +1340,7 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="22">
@@ -1348,7 +1348,7 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="23">
@@ -1356,7 +1356,7 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="24">
@@ -1364,7 +1364,7 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="25">
@@ -1372,7 +1372,7 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="26">
@@ -1380,7 +1380,7 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="27">
@@ -1388,7 +1388,7 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="28">
@@ -1396,7 +1396,7 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="29">
@@ -1404,7 +1404,7 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="30">
@@ -1525,7 +1525,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12">
@@ -1533,7 +1533,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13">
@@ -1541,7 +1541,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="14">
@@ -1549,7 +1549,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="15">
@@ -1581,7 +1581,7 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="19">
@@ -1613,7 +1613,7 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="23">
@@ -1621,7 +1621,7 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="24">
@@ -1629,7 +1629,7 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="25">
@@ -1637,7 +1637,7 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="26">
@@ -1645,7 +1645,7 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="27">
@@ -1653,7 +1653,7 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="28">
@@ -1661,7 +1661,7 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="29">
@@ -1669,7 +1669,7 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="30">
@@ -1790,7 +1790,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12">
@@ -1798,7 +1798,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13">
@@ -1806,7 +1806,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="14">
@@ -1814,7 +1814,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="15">
@@ -1878,7 +1878,7 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="23">
@@ -1886,7 +1886,7 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="24">
@@ -1902,7 +1902,7 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="26">
@@ -1910,7 +1910,7 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="27">
@@ -1918,7 +1918,7 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="28">
@@ -1926,7 +1926,7 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="29">
@@ -1934,7 +1934,7 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="30">
@@ -2055,7 +2055,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12">
@@ -2063,7 +2063,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13">
@@ -2071,7 +2071,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="14">
@@ -2103,7 +2103,7 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="18">
@@ -2119,7 +2119,7 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="20">
@@ -2143,7 +2143,7 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="23">
@@ -2159,7 +2159,7 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="25">
@@ -2167,7 +2167,7 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="26">
@@ -2175,7 +2175,7 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="27">
@@ -2183,7 +2183,7 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="28">
@@ -2191,7 +2191,7 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="29">
@@ -2199,7 +2199,7 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="30">
@@ -2207,7 +2207,7 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="31">
@@ -2320,7 +2320,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12">
@@ -2328,7 +2328,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13">
@@ -2336,7 +2336,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="14">
@@ -2344,7 +2344,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="15">
@@ -2368,7 +2368,7 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="18">
@@ -2384,7 +2384,7 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="20">
@@ -2392,7 +2392,7 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="21">
@@ -2424,7 +2424,7 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="25">
@@ -2440,7 +2440,7 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="27">
@@ -2448,7 +2448,7 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="28">
@@ -2456,7 +2456,7 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="29">
@@ -2464,7 +2464,7 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="30">
@@ -2472,7 +2472,7 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="31">
@@ -2585,7 +2585,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12">
@@ -2593,7 +2593,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13">
@@ -2601,7 +2601,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="14">
@@ -2609,7 +2609,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="15">
@@ -2633,7 +2633,7 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="18">
@@ -2641,7 +2641,7 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="19">
@@ -2649,7 +2649,7 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="20">
@@ -2657,7 +2657,7 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="21">
@@ -2665,7 +2665,7 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="22">
@@ -2673,7 +2673,7 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="23">
@@ -2713,7 +2713,7 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="28">
@@ -2729,7 +2729,7 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="30">
@@ -2737,7 +2737,7 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="31">
@@ -2850,7 +2850,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>47</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12">
@@ -2858,7 +2858,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13">
@@ -2866,7 +2866,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="14">
@@ -2874,7 +2874,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="15">
@@ -2882,7 +2882,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="16">
@@ -2890,7 +2890,7 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="17">
@@ -2922,7 +2922,7 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="21">
@@ -2930,7 +2930,7 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="22">
@@ -2938,7 +2938,7 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="23">
@@ -2946,7 +2946,7 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="24">
@@ -2954,7 +2954,7 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="25">
@@ -2970,7 +2970,7 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="27">
@@ -3002,7 +3002,7 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="31">
@@ -3010,7 +3010,7 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -3107,7 +3107,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11">
@@ -3115,7 +3115,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>51</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12">
@@ -3123,7 +3123,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>56</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13">
@@ -3131,7 +3131,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>60</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14">
@@ -3139,7 +3139,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="15">
@@ -3147,7 +3147,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="16">
@@ -3155,7 +3155,7 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="17">
@@ -3163,7 +3163,7 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="18">
@@ -3187,7 +3187,7 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="21">
@@ -3203,7 +3203,7 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="23">
@@ -3211,7 +3211,7 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="24">
@@ -3219,7 +3219,7 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="25">
@@ -3227,7 +3227,7 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="26">
@@ -3235,7 +3235,7 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="27">
@@ -3243,7 +3243,7 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="28">
@@ -3251,7 +3251,7 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="29">
@@ -3259,7 +3259,7 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="30">
@@ -3267,7 +3267,7 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="31">
@@ -3380,7 +3380,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12">
@@ -3388,7 +3388,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13">
@@ -3396,7 +3396,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="14">
@@ -3404,7 +3404,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="15">
@@ -3412,7 +3412,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="16">
@@ -3420,7 +3420,7 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="17">
@@ -3428,7 +3428,7 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="18">
@@ -3436,7 +3436,7 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="19">
@@ -3476,7 +3476,7 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="24">
@@ -3484,7 +3484,7 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>124</v>
+        <v>126</v>
       </c>
     </row>
     <row r="25">
@@ -3492,7 +3492,7 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="26">
@@ -3621,7 +3621,7 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9">
@@ -3629,7 +3629,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>48</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10">
@@ -3637,7 +3637,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>53</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11">
@@ -3645,7 +3645,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>57</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12">
@@ -3653,7 +3653,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>61</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13">
@@ -3661,7 +3661,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>64</v>
+        <v>51</v>
       </c>
     </row>
     <row r="14">
@@ -3669,7 +3669,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>67</v>
+        <v>57</v>
       </c>
     </row>
     <row r="15">
@@ -3677,7 +3677,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>71</v>
+        <v>63</v>
       </c>
     </row>
     <row r="16">
@@ -3685,7 +3685,7 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>74</v>
+        <v>67</v>
       </c>
     </row>
     <row r="17">
@@ -3693,7 +3693,7 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="18">
@@ -3701,7 +3701,7 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="19">
@@ -3709,7 +3709,7 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="20">
@@ -3717,7 +3717,7 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="21">
@@ -3725,7 +3725,7 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="22">
@@ -3757,7 +3757,7 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="26">
@@ -3765,7 +3765,7 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="27">
@@ -3773,7 +3773,7 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="28">
@@ -3781,7 +3781,7 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="29">
@@ -3789,7 +3789,7 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="30">
@@ -3797,7 +3797,7 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row r="31">
@@ -3805,7 +3805,7 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -3910,7 +3910,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12">
@@ -3918,7 +3918,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13">
@@ -3926,7 +3926,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14">
@@ -3934,7 +3934,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="15">
@@ -3942,7 +3942,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="16">
@@ -3950,7 +3950,7 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="17">
@@ -3958,7 +3958,7 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="18">
@@ -3974,7 +3974,7 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="20">
@@ -4006,7 +4006,7 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="24">
@@ -4014,7 +4014,7 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="25">
@@ -4022,7 +4022,7 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="26">
@@ -4175,7 +4175,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12">
@@ -4183,7 +4183,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="13">
@@ -4191,7 +4191,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="14">
@@ -4199,7 +4199,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="15">
@@ -4207,7 +4207,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="16">
@@ -4215,7 +4215,7 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="17">
@@ -4223,7 +4223,7 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="18">
@@ -4231,7 +4231,7 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="19">
@@ -4239,7 +4239,7 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="20">
@@ -4247,7 +4247,7 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="21">
@@ -4279,7 +4279,7 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="25">
@@ -4287,7 +4287,7 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="26">
@@ -4295,7 +4295,7 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="27">
@@ -4440,7 +4440,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12">
@@ -4448,7 +4448,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="13">
@@ -4456,7 +4456,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="14">
@@ -4464,7 +4464,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="15">
@@ -4472,7 +4472,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="16">
@@ -4480,7 +4480,7 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="17">
@@ -4488,7 +4488,7 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="18">
@@ -4496,7 +4496,7 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="19">
@@ -4504,7 +4504,7 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="20">
@@ -4512,7 +4512,7 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="21">
@@ -4520,7 +4520,7 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="22">
@@ -4544,7 +4544,7 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="25">
@@ -4705,7 +4705,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12">
@@ -4713,7 +4713,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="13">
@@ -4721,7 +4721,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="14">
@@ -4729,7 +4729,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="15">
@@ -4737,7 +4737,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="16">
@@ -4745,7 +4745,7 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="17">
@@ -4753,7 +4753,7 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="18">
@@ -4761,7 +4761,7 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="19">
@@ -4769,7 +4769,7 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="20">
@@ -4777,7 +4777,7 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="21">
@@ -4785,7 +4785,7 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="22">
@@ -4793,7 +4793,7 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="23">
@@ -4970,7 +4970,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12">
@@ -4978,7 +4978,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13">
@@ -4986,7 +4986,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="14">
@@ -4994,7 +4994,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="15">
@@ -5002,7 +5002,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="16">
@@ -5010,7 +5010,7 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="17">
@@ -5018,7 +5018,7 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="18">
@@ -5026,7 +5026,7 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="19">
@@ -5034,7 +5034,7 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="20">
@@ -5042,7 +5042,7 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="21">
@@ -5050,7 +5050,7 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="22">
@@ -5066,7 +5066,7 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="24">
@@ -5082,7 +5082,7 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="26">
@@ -5235,7 +5235,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12">
@@ -5243,7 +5243,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="13">
@@ -5251,7 +5251,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="14">
@@ -5259,7 +5259,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="15">
@@ -5267,7 +5267,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="16">
@@ -5275,7 +5275,7 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="17">
@@ -5283,7 +5283,7 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="18">
@@ -5291,7 +5291,7 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="19">
@@ -5299,7 +5299,7 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="20">
@@ -5307,7 +5307,7 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="21">
@@ -5315,7 +5315,7 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="22">
@@ -5323,7 +5323,7 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="23">
@@ -5331,7 +5331,7 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="24">
@@ -5339,7 +5339,7 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="25">
@@ -5355,7 +5355,7 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="27">
@@ -5363,7 +5363,7 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="28">
@@ -5500,7 +5500,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12">
@@ -5508,7 +5508,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="13">
@@ -5516,7 +5516,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="14">
@@ -5524,7 +5524,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="15">
@@ -5532,7 +5532,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="16">
@@ -5540,7 +5540,7 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="17">
@@ -5548,7 +5548,7 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="18">
@@ -5556,7 +5556,7 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="19">
@@ -5564,7 +5564,7 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="20">
@@ -5572,7 +5572,7 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="21">
@@ -5580,7 +5580,7 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="22">
@@ -5588,7 +5588,7 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="23">
@@ -5596,7 +5596,7 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="24">
@@ -5604,7 +5604,7 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="25">
@@ -5612,7 +5612,7 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="26">
@@ -5628,7 +5628,7 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="28">
@@ -5636,7 +5636,7 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="29">

</xml_diff>